<commit_message>
continue LZ tree code
</commit_message>
<xml_diff>
--- a/src/table1.xlsx
+++ b/src/table1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bm\Desktop\matlab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bm\Desktop\Developing-Variety-Of-Methods-For-Identifying-Anomalies-\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>id</t>
   </si>
@@ -32,13 +32,10 @@
     <t>age</t>
   </si>
   <si>
-    <t>blood</t>
+    <t>sugarBlood</t>
   </si>
   <si>
-    <t>dofek</t>
-  </si>
-  <si>
-    <t>check</t>
+    <t>pulse</t>
   </si>
 </sst>
 </file>
@@ -391,15 +388,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC74904-0112-4737-9E34-1F90110ADB6C}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,11 +409,8 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -429,11 +423,8 @@
       <c r="D2">
         <v>20</v>
       </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -446,11 +437,8 @@
       <c r="D3">
         <v>50</v>
       </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -463,11 +451,8 @@
       <c r="D4">
         <v>30</v>
       </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -480,11 +465,8 @@
       <c r="D5">
         <v>25</v>
       </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -497,11 +479,8 @@
       <c r="D6">
         <v>40</v>
       </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -514,11 +493,8 @@
       <c r="D7">
         <v>20</v>
       </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -531,11 +507,8 @@
       <c r="D8">
         <v>25</v>
       </c>
-      <c r="E8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -548,11 +521,8 @@
       <c r="D9">
         <v>23</v>
       </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -565,11 +535,8 @@
       <c r="D10">
         <v>31</v>
       </c>
-      <c r="E10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -582,8 +549,103 @@
       <c r="D11">
         <v>50</v>
       </c>
-      <c r="E11">
-        <v>4</v>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="C12">
+        <v>80</v>
+      </c>
+      <c r="D12">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>61</v>
+      </c>
+      <c r="C13">
+        <v>88</v>
+      </c>
+      <c r="D13">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>72</v>
+      </c>
+      <c r="C14">
+        <v>78</v>
+      </c>
+      <c r="D14">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>82</v>
+      </c>
+      <c r="C15">
+        <v>76</v>
+      </c>
+      <c r="D15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>115</v>
+      </c>
+      <c r="C16">
+        <v>86</v>
+      </c>
+      <c r="D16">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>70</v>
+      </c>
+      <c r="C17">
+        <v>68</v>
+      </c>
+      <c r="D17">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>56</v>
+      </c>
+      <c r="C18">
+        <v>84</v>
+      </c>
+      <c r="D18">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>